<commit_message>
quotation document update# Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/程序员客栈项目/因卓科技教育平台/因卓教育阶段二/软件开发/输入文档/11.30因卓教育阶段二项目计划.xlsx
+++ b/程序员客栈项目/因卓科技教育平台/因卓教育阶段二/软件开发/输入文档/11.30因卓教育阶段二项目计划.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="18084"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="18084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="项目说明" sheetId="1" r:id="rId1"/>
@@ -4761,7 +4761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:IW32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -9657,8 +9657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:IW49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:O49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" customHeight="1"/>

</xml_diff>